<commit_message>
qarsf migration and sydata test cases
</commit_message>
<xml_diff>
--- a/templates/QARSF/RSTK8065-Consolidated Sales Order Fulfillment-AllProductTypes - SOAPI.xlsx
+++ b/templates/QARSF/RSTK8065-Consolidated Sales Order Fulfillment-AllProductTypes - SOAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Automation_1Updated\rsqasampleproj\templates\QARSF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7A87BD-B20C-4BBB-B871-050B4CFD4858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D440FEE-0995-42C9-BC1D-13452A39C124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="20460" windowHeight="10890" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddLine" sheetId="15" r:id="rId1"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +929,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C60F850-BC07-45D7-8A71-F5FA33E22AE5}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F9AC43-F5C0-448B-A649-9DBCCD7B9161}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>